<commit_message>
폭신 작업 완료, damage_display 완료
</commit_message>
<xml_diff>
--- a/기획서/스킬 레벨링.xlsx
+++ b/기획서/스킬 레벨링.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNITY\UNITY\Slave revolution\기획서\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7710" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="마족 스킬" sheetId="1" r:id="rId1"/>
@@ -1229,7 +1234,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1239,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1522,12 +1527,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1610,7 +1614,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>121</v>
       </c>
@@ -1753,7 +1757,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="26.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>125</v>
       </c>
@@ -1975,13 +1979,7 @@
       <c r="D39" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G20">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="동은"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G20"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
hp system 속성 추
</commit_message>
<xml_diff>
--- a/기획서/스킬 레벨링.xlsx
+++ b/기획서/스킬 레벨링.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gg\기획서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNITY\UNITY\Slave revolution\기획서\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="마족 스킬" sheetId="1" r:id="rId1"/>
@@ -1276,9 +1276,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1571,12 +1571,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H17" sqref="H17"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1659,7 +1658,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>112</v>
       </c>
@@ -1725,7 +1724,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>113</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="26.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>116</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="25.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
         <v>125</v>
       </c>
@@ -2045,13 +2044,7 @@
       <c r="D39" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H20">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="동은"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H20"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>